<commit_message>
added data type tab
</commit_message>
<xml_diff>
--- a/files/Data-Prod Map.xlsx
+++ b/files/Data-Prod Map.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Direct+ Data-Product Mapping" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Types" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8491" uniqueCount="1873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8503" uniqueCount="1885">
   <si>
     <t>Element Key</t>
   </si>
@@ -5741,12 +5742,49 @@
   <si>
     <t>The classification of the entity based on the age of the entity.</t>
   </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>All string fields are supported by UTF-8 characters.</t>
+  </si>
+  <si>
+    <t>Unless otherwise specified in the documentation, the following standards apply to data types:</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Date/time</t>
+  </si>
+  <si>
+    <t>Value: true, false, null</t>
+  </si>
+  <si>
+    <t>Format: YYYY-MM-DDThh:mm:ss.sTZD
+The date and time, in ISO 8601 UTC Z standard in GMT</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5758,6 +5796,14 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFEBF5F9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5822,7 +5868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5835,6 +5881,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6196,52 +6251,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5" t="s">
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
     </row>
     <row r="2" spans="1:21" ht="33.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
       <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
@@ -34322,4 +34377,88 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.08984375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="42.81640625" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>1873</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1874</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>1876</v>
+      </c>
+      <c r="B3" s="5">
+        <v>256</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>1879</v>
+      </c>
+      <c r="B4" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B5" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>1881</v>
+      </c>
+      <c r="B6" s="5">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>1882</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>1884</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>